<commit_message>
retidying repo (again), including fabricio extraction in full analysis
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /acclimation /acclimation7jun21.xlsx
+++ b/data extraction /lit search metadata /acclimation /acclimation7jun21.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /acclimation /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228924F6-224D-FB4A-BE3D-81CCE34BC4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B413B7-6B96-484E-9205-48A8BC1B42FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23560" windowHeight="10000" xr2:uid="{15E522D6-79C7-664C-9C48-CC1A91CDC4AD}"/>
+    <workbookView xWindow="28800" yWindow="-28000" windowWidth="23560" windowHeight="12660" xr2:uid="{15E522D6-79C7-664C-9C48-CC1A91CDC4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$T$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$T$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="150">
   <si>
     <t>Bartheld_2017_JOOFTHBI</t>
   </si>
@@ -150,21 +150,6 @@
     <t>JOURNAL OF EVOLUTIONARY BIOLOGY</t>
   </si>
   <si>
-    <t>Fabricio.Neto_2019_JOOFTHBI</t>
-  </si>
-  <si>
-    <t>Fabricio-Neto, Ailton and Bueno Gavira, Rodrigo Samuel and Andrade, Denis Vieira</t>
-  </si>
-  <si>
-    <t>Thermal regime effects on the resting metabolic rate of rattlesnakes depend on temperature range</t>
-  </si>
-  <si>
-    <t>10.1016/j.jtherbio.2019.05.025</t>
-  </si>
-  <si>
-    <t>While ectothermic organisms often experience considerable circadian variation in body temperature under natural conditions, the study of the effects of temperature on metabolic rates are traditionally based on subjecting animals to constant temperature regimes. Whether data resulting from constant-temperature experiments accurately predicts temperature effects under more natural fluctuating temperature regimes remains uncertain. To address such possibility, we measured the resting metabolic rates of the South American rattlesnakes (Crotalus durissus) under constant and circadian fluctuating thermal regimes in a range of temperatures. Metabolic rates measured at constant 20 degrees C and 25 degrees C did not differ from the rates measured at fluctuating regimes with corresponding mean temperatures. However, the difference between thermal regimes increased with temperature, with the metabolic rate measured at constant 30 degrees C being greater than that measured at the fluctuating thermal regime with corresponding mean temperature. Therefore, our results indicate that thermal regime effects on rattlesnakes' metabolism is dependent on temperature range. Broadly, our results highlight the importance of considering multi-factorial attributes of temperature variation in the exam of its effects over functional traits. Such approach provides a more solid support for inferences about temperature effects on the life history, ecology and conservation of ectothermic organisms.</t>
-  </si>
-  <si>
     <t>Hallsson_2012_JOOFEVBI</t>
   </si>
   <si>
@@ -310,9 +295,6 @@
   </si>
   <si>
     <t xml:space="preserve">heatshock assay--likely not usable for acclimation, excluded because mean temperature not the same for flux and constant trt </t>
-  </si>
-  <si>
-    <t>acclimated at fluctuating and exposed to different constant treatments, not sure how to handle the isolated thermoperiod trts (no supp info or explanation in the methods)</t>
   </si>
   <si>
     <t>table 1</t>
@@ -869,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8F4095-DAD1-314E-93A6-2C3D1771AF66}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -924,7 +906,7 @@
         <v>25</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -971,30 +953,30 @@
         <v>8</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F3" s="3">
         <v>2014</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>6</v>
@@ -1006,24 +988,24 @@
         <v>32</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
@@ -1053,42 +1035,42 @@
         <v>32</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F5" s="3">
         <v>2018</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>6</v>
@@ -1100,42 +1082,42 @@
         <v>32</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F6" s="3">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>6</v>
@@ -1147,86 +1129,80 @@
         <v>8</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="3">
-        <v>2020</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="C7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>107</v>
+      <c r="I7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F8" s="4">
         <v>2016</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>6</v>
@@ -1237,34 +1213,37 @@
       <c r="J8" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="K8" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="M8" s="4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F9" s="4">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>6</v>
@@ -1276,36 +1255,36 @@
         <v>8</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F10" s="4">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>6</v>
@@ -1317,36 +1296,36 @@
         <v>8</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F11" s="4">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>6</v>
@@ -1358,13 +1337,13 @@
         <v>8</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>130</v>
+        <v>38</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>131</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1378,16 +1357,16 @@
         <v>134</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F12" s="4">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>6</v>
@@ -1399,36 +1378,36 @@
         <v>8</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F13" s="4">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>6</v>
@@ -1440,168 +1419,171 @@
         <v>8</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>105</v>
+        <v>145</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2012</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F14" s="4">
-        <v>2009</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F15" s="2">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="N15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="O15" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F16" s="2">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="F17" s="2">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>6</v>
@@ -1613,39 +1595,42 @@
         <v>9</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>154</v>
+        <v>88</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="F18" s="2">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>6</v>
@@ -1657,74 +1642,27 @@
         <v>9</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>93</v>
+        <v>149</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="2">
-        <v>2017</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:T22" xr:uid="{EA640836-B94E-084A-8D12-EC9660F9218A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T20">
-    <sortCondition descending="1" ref="J2:J20"/>
-    <sortCondition descending="1" ref="O2:O20"/>
-    <sortCondition ref="A2:A20"/>
+  <autoFilter ref="A2:T21" xr:uid="{EA640836-B94E-084A-8D12-EC9660F9218A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T19">
+    <sortCondition descending="1" ref="J2:J19"/>
+    <sortCondition descending="1" ref="O2:O19"/>
+    <sortCondition ref="A2:A19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reorganizing repo and creating data vis file for manuscript data analysis
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /acclimation /acclimation7jun21.xlsx
+++ b/data extraction /lit search metadata /acclimation /acclimation7jun21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /acclimation /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336C37F2-4A33-7D4A-8699-EBC2929D5777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E9B3B0-DBEC-2A49-A3E9-DC55004E5853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-28000" windowWidth="23560" windowHeight="12660" xr2:uid="{15E522D6-79C7-664C-9C48-CC1A91CDC4AD}"/>
   </bookViews>
@@ -414,9 +414,6 @@
     <t>We investigated the effects of constant and diel-fluctuating temperature acclimation on the thermal tolerance, swimming capacity, specific dynamic action (SDA) and growth performance of juvenile Chinese bream (Parabramis pekinensis). The critical thermal maxima (CTmax), critical thermal minima (CTmin), lethal thermal maxima (LTmax), lethal thermal minima (LTmin), critical swimming speed (Ucrit) and fast-start escape response after 30d acclimation to three constant temperatures (15, 20 and 25C) and one diel-fluctuating temperature (205C) were measured. In addition, feeding rate (FR), feeding efficiency (FE) and specific growth rate (SGR) were measured. The diel-fluctuating temperature group showed lower CTmin than the 20C group but a similar CTmax, indicating a wider thermal scope. SDA linearly increased with the temperature. Temperature variation between 20 and 25C had little effect on either swimming or growth performance. However, fish in the 15C group exhibited much poorer swimming and growth performance than those in the 20C group. Ucrit decreased slightly under low acclimation temperature due to the pronounced improvement in swimming efficiency under cold temperature. Fish in the diel-fluctuating temperature group fed more but exhibited similar SGR compared to 20C group, possibly due in part to an increase in energy expenditure to cope with the temperature fluctuation. The narrower thermal scope and lower CTmax of Chinese bream together with the conservation of CTmax with temperature acclimation, suggests that local water temperature elevations may have more profound effects on Chinese bream than on other fish species in the Three Gorges Reservoir.  2014 Elsevier Inc.</t>
   </si>
   <si>
-    <t xml:space="preserve"> this features multiple generations-- generation time is 25 day at 30 C; excluded because the fluctuating treatment does not match the constant treatment and therefore, cannot be paired…</t>
-  </si>
-  <si>
     <t>flux and constant don't have the same mean and they are not the same flux pattern (trt exposed to multiple flux patterns)</t>
   </si>
   <si>
@@ -466,6 +463,9 @@
   </si>
   <si>
     <t>full analysis for figure 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> this features multiple generations-- generation time is 25 day at 30 C; excluded because the fluctuating treatment mean does not match the constant treatment and therefore, cannot be paired…</t>
   </si>
 </sst>
 </file>
@@ -842,7 +842,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1164,10 +1164,10 @@
         <v>8</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>99</v>
@@ -1255,13 +1255,13 @@
         <v>8</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>8</v>
@@ -1316,25 +1316,25 @@
     </row>
     <row r="11" spans="1:15" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>143</v>
       </c>
       <c r="F11" s="4">
         <v>2020</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>6</v>
@@ -1346,10 +1346,10 @@
         <v>8</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>8</v>
@@ -1390,10 +1390,10 @@
         <v>8</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>8</v>
@@ -1440,7 +1440,7 @@
         <v>46</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>76</v>
@@ -1487,7 +1487,7 @@
         <v>11</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>76</v>
@@ -1534,7 +1534,7 @@
         <v>11</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>76</v>
@@ -1628,7 +1628,7 @@
         <v>11</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
updates and removing non-normally distributed data
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /acclimation /acclimation7jun21.xlsx
+++ b/data extraction /lit search metadata /acclimation /acclimation7jun21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /acclimation /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E9B3B0-DBEC-2A49-A3E9-DC55004E5853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C96BC7-4366-D249-97DA-F1D59E3F7FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-28000" windowWidth="23560" windowHeight="12660" xr2:uid="{15E522D6-79C7-664C-9C48-CC1A91CDC4AD}"/>
   </bookViews>
@@ -435,9 +435,6 @@
     <t xml:space="preserve">not sure how to handle constant mean with changing variance….so far, just extracted constant mean and constant variance trts as paired </t>
   </si>
   <si>
-    <t xml:space="preserve">not sure how to handle the data where they include and exclude individuals with different thermal preferences; decided to just use all individuals and not the exclusion analysis because I would be representing a lot of data twice and that might skew the data; extracted all data from figure 1 but not sure whether I should be including thermal preference data the both includes or excludes ctmin; assumed median values as means here </t>
-  </si>
-  <si>
     <t xml:space="preserve">acclimation; excluded the figures/data that reported the fluctuating treatments at the two different min/max. </t>
   </si>
   <si>
@@ -466,6 +463,9 @@
   </si>
   <si>
     <t xml:space="preserve"> this features multiple generations-- generation time is 25 day at 30 C; excluded because the fluctuating treatment mean does not match the constant treatment and therefore, cannot be paired…</t>
+  </si>
+  <si>
+    <t>not sure how to handle the data where they include and exclude individuals with different thermal preferences; decided to just use all individuals and not the exclusion analysis because I would be representing a lot of data twice and that might skew the data; extracted all data from figure 1 but not sure whether I should be including thermal preference data the both includes or excludes ctmin; assumed median values as means here; excluded some data from figure 1, figure 3a because it was not normally distributed</t>
   </si>
 </sst>
 </file>
@@ -842,7 +842,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1258,7 +1258,7 @@
         <v>133</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>132</v>
@@ -1316,25 +1316,25 @@
     </row>
     <row r="11" spans="1:15" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="F11" s="4">
         <v>2020</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>6</v>
@@ -1346,10 +1346,10 @@
         <v>8</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>8</v>
@@ -1390,10 +1390,10 @@
         <v>8</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>8</v>
@@ -1440,7 +1440,7 @@
         <v>46</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>76</v>

</xml_diff>